<commit_message>
wip calculate vehicle costs
</commit_message>
<xml_diff>
--- a/calculators/vehicle-calculator.xlsx
+++ b/calculators/vehicle-calculator.xlsx
@@ -32,35 +32,57 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">This includes all weapons on the vehicle, additional modifiers like open topped or coaxial are deduced later.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C74" authorId="0">
+    <comment ref="C76" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">In historical scenarios, there might be additional modifiers other than the hard factors like loadout.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C79" authorId="0">
+    <comment ref="C81" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Keep in mind that units from this calculator represent the stock option. Other weapons might be added on later as optional weapons and rules.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">JSFT 20pt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O75" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">EW System 20pt
+</t>
         </r>
       </text>
     </comment>
@@ -69,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t xml:space="preserve">H.E.A.T. Vehicle Cost Calculator Sheet v1.0</t>
   </si>
@@ -98,6 +120,9 @@
     <t xml:space="preserve">Eurocopter</t>
   </si>
   <si>
+    <t xml:space="preserve">M113 mortar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wiesel I Mörser 120mm </t>
   </si>
   <si>
@@ -407,6 +432,9 @@
     <t xml:space="preserve">Slow</t>
   </si>
   <si>
+    <t xml:space="preserve">Spotter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slow Load</t>
   </si>
   <si>
@@ -429,6 +457,9 @@
   </si>
   <si>
     <t xml:space="preserve">Coaxial weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Rule</t>
   </si>
   <si>
     <t xml:space="preserve">Historical costs</t>
@@ -459,10 +490,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -495,6 +527,11 @@
       <name val="Cascadia Code SemiBold"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -588,7 +625,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,10 +694,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -673,7 +706,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,59 +833,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:DF81"/>
+  <dimension ref="C2:DG87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="0" topLeftCell="G31" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
-      <selection pane="topRight" activeCell="H54" activeCellId="0" sqref="H54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="0" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="AB62" activeCellId="0" sqref="AB62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="19.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="30.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="27.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="38" style="0" width="2.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="25.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="40.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="19.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="23.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="30.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="27.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="39" style="1" width="2.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="J1" s="1"/>
-    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -860,19 +887,15 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
-      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
-      <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
@@ -978,7 +1001,9 @@
       <c r="AK4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AL4" s="7"/>
+      <c r="AL4" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
@@ -995,7 +1020,7 @@
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
       <c r="BB4" s="7"/>
-      <c r="BC4" s="9"/>
+      <c r="BC4" s="7"/>
       <c r="BD4" s="9"/>
       <c r="BE4" s="9"/>
       <c r="BF4" s="9"/>
@@ -1051,14 +1076,14 @@
       <c r="DD4" s="9"/>
       <c r="DE4" s="9"/>
       <c r="DF4" s="9"/>
+      <c r="DG4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
       <c r="C5" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" s="9" t="n">
         <v>15</v>
@@ -1168,12 +1193,12 @@
       <c r="DD5" s="9"/>
       <c r="DE5" s="9"/>
       <c r="DF5" s="9"/>
+      <c r="DG5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
       <c r="C6" s="10"/>
       <c r="D6" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>50</v>
@@ -1192,22 +1217,54 @@
       <c r="K6" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
+      <c r="L6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="R6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9"/>
@@ -1291,12 +1348,12 @@
       <c r="DD6" s="9"/>
       <c r="DE6" s="9"/>
       <c r="DF6" s="9"/>
+      <c r="DG6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
       <c r="C7" s="10"/>
       <c r="D7" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E7" s="9" t="n">
         <v>70</v>
@@ -1323,7 +1380,9 @@
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
+      <c r="AB7" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC7" s="9"/>
       <c r="AD7" s="9"/>
       <c r="AE7" s="9"/>
@@ -1406,12 +1465,12 @@
       <c r="DD7" s="9"/>
       <c r="DE7" s="9"/>
       <c r="DF7" s="9"/>
+      <c r="DG7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>110</v>
@@ -1523,12 +1582,12 @@
       <c r="DD8" s="9"/>
       <c r="DE8" s="9"/>
       <c r="DF8" s="9"/>
+      <c r="DG8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="9" t="n">
         <v>190</v>
@@ -1638,12 +1697,12 @@
       <c r="DD9" s="9"/>
       <c r="DE9" s="9"/>
       <c r="DF9" s="9"/>
+      <c r="DG9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
       <c r="C10" s="10"/>
       <c r="D10" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="9" t="n">
         <v>350</v>
@@ -1753,14 +1812,14 @@
       <c r="DD10" s="9"/>
       <c r="DE10" s="9"/>
       <c r="DF10" s="9"/>
+      <c r="DG10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
       <c r="C11" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="9" t="n">
         <v>5</v>
@@ -1870,12 +1929,12 @@
       <c r="DD11" s="9"/>
       <c r="DE11" s="9"/>
       <c r="DF11" s="9"/>
+      <c r="DG11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E12" s="9" t="n">
         <v>10</v>
@@ -1985,12 +2044,12 @@
       <c r="DD12" s="9"/>
       <c r="DE12" s="9"/>
       <c r="DF12" s="9"/>
+      <c r="DG12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="9" t="n">
         <v>20</v>
@@ -2100,12 +2159,12 @@
       <c r="DD13" s="9"/>
       <c r="DE13" s="9"/>
       <c r="DF13" s="9"/>
+      <c r="DG13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" s="9" t="n">
         <v>40</v>
@@ -2215,12 +2274,12 @@
       <c r="DD14" s="9"/>
       <c r="DE14" s="9"/>
       <c r="DF14" s="9"/>
+      <c r="DG14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="9" t="n">
         <v>80</v>
@@ -2330,12 +2389,12 @@
       <c r="DD15" s="9"/>
       <c r="DE15" s="9"/>
       <c r="DF15" s="9"/>
+      <c r="DG15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
       <c r="C16" s="10"/>
       <c r="D16" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="9" t="n">
         <v>120</v>
@@ -2445,12 +2504,12 @@
       <c r="DD16" s="9"/>
       <c r="DE16" s="9"/>
       <c r="DF16" s="9"/>
+      <c r="DG16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
       <c r="C17" s="10"/>
       <c r="D17" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="9" t="n">
         <v>-10</v>
@@ -2560,14 +2619,14 @@
       <c r="DD17" s="9"/>
       <c r="DE17" s="9"/>
       <c r="DF17" s="9"/>
+      <c r="DG17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
       <c r="C18" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E18" s="9" t="n">
         <v>25</v>
@@ -2677,12 +2736,12 @@
       <c r="DD18" s="9"/>
       <c r="DE18" s="9"/>
       <c r="DF18" s="9"/>
+      <c r="DG18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
       <c r="C19" s="10"/>
       <c r="D19" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E19" s="9" t="n">
         <v>40</v>
@@ -2794,12 +2853,12 @@
       <c r="DD19" s="9"/>
       <c r="DE19" s="9"/>
       <c r="DF19" s="9"/>
+      <c r="DG19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
       <c r="C20" s="10"/>
       <c r="D20" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E20" s="9" t="n">
         <v>55</v>
@@ -2909,12 +2968,12 @@
       <c r="DD20" s="9"/>
       <c r="DE20" s="9"/>
       <c r="DF20" s="9"/>
+      <c r="DG20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
       <c r="C21" s="10"/>
       <c r="D21" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E21" s="9" t="n">
         <v>60</v>
@@ -3024,14 +3083,14 @@
       <c r="DD21" s="9"/>
       <c r="DE21" s="9"/>
       <c r="DF21" s="9"/>
+      <c r="DG21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
       <c r="C22" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E22" s="9" t="n">
         <v>2</v>
@@ -3046,19 +3105,45 @@
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
+      <c r="P22" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="R22" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="S22" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="T22" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="U22" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="V22" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="W22" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="X22" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y22" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z22" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA22" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB22" s="9" t="n">
+        <v>6</v>
+      </c>
       <c r="AC22" s="9"/>
       <c r="AD22" s="9"/>
       <c r="AE22" s="9"/>
@@ -3141,14 +3226,14 @@
       <c r="DD22" s="9"/>
       <c r="DE22" s="9"/>
       <c r="DF22" s="9"/>
+      <c r="DG22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
       <c r="C23" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E23" s="9" t="n">
         <v>5</v>
@@ -3258,12 +3343,12 @@
       <c r="DD23" s="9"/>
       <c r="DE23" s="9"/>
       <c r="DF23" s="9"/>
+      <c r="DG23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
       <c r="C24" s="16"/>
       <c r="D24" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" s="9" t="n">
         <v>10</v>
@@ -3291,8 +3376,12 @@
       <c r="X24" s="9"/>
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
+      <c r="AA24" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC24" s="9"/>
       <c r="AD24" s="9"/>
       <c r="AE24" s="9"/>
@@ -3375,12 +3464,12 @@
       <c r="DD24" s="9"/>
       <c r="DE24" s="9"/>
       <c r="DF24" s="9"/>
+      <c r="DG24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0"/>
       <c r="C25" s="16"/>
       <c r="D25" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E25" s="9" t="n">
         <v>20</v>
@@ -3490,18 +3579,18 @@
       <c r="DD25" s="9"/>
       <c r="DE25" s="9"/>
       <c r="DF25" s="9"/>
+      <c r="DG25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
       <c r="C26" s="16"/>
       <c r="D26" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="9" t="n">
         <v>20</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -3607,12 +3696,12 @@
       <c r="DD26" s="9"/>
       <c r="DE26" s="9"/>
       <c r="DF26" s="9"/>
+      <c r="DG26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
       <c r="C27" s="16"/>
       <c r="D27" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" s="9" t="n">
         <v>20</v>
@@ -3722,18 +3811,18 @@
       <c r="DD27" s="9"/>
       <c r="DE27" s="9"/>
       <c r="DF27" s="9"/>
+      <c r="DG27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0"/>
       <c r="C28" s="16"/>
       <c r="D28" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E28" s="9" t="n">
         <v>30</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -3755,7 +3844,9 @@
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
+      <c r="AA28" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AB28" s="9"/>
       <c r="AC28" s="9"/>
       <c r="AD28" s="9"/>
@@ -3839,18 +3930,18 @@
       <c r="DD28" s="9"/>
       <c r="DE28" s="9"/>
       <c r="DF28" s="9"/>
+      <c r="DG28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0"/>
       <c r="C29" s="16"/>
       <c r="D29" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E29" s="9" t="n">
         <v>40</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3875,7 +3966,9 @@
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
-      <c r="AB29" s="9"/>
+      <c r="AB29" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC29" s="9"/>
       <c r="AD29" s="9"/>
       <c r="AE29" s="9"/>
@@ -3958,18 +4051,18 @@
       <c r="DD29" s="9"/>
       <c r="DE29" s="9"/>
       <c r="DF29" s="9"/>
+      <c r="DG29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0"/>
       <c r="C30" s="16"/>
       <c r="D30" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E30" s="9" t="n">
         <v>50</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
@@ -4075,18 +4168,18 @@
       <c r="DD30" s="9"/>
       <c r="DE30" s="9"/>
       <c r="DF30" s="9"/>
+      <c r="DG30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
       <c r="C31" s="16"/>
       <c r="D31" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E31" s="9" t="n">
         <v>50</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
@@ -4192,18 +4285,18 @@
       <c r="DD31" s="9"/>
       <c r="DE31" s="9"/>
       <c r="DF31" s="9"/>
+      <c r="DG31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
       <c r="C32" s="16"/>
       <c r="D32" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E32" s="9" t="n">
         <v>70</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -4309,18 +4402,18 @@
       <c r="DD32" s="9"/>
       <c r="DE32" s="9"/>
       <c r="DF32" s="9"/>
+      <c r="DG32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0"/>
       <c r="C33" s="16"/>
       <c r="D33" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E33" s="9" t="n">
         <v>110</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G33" s="9" t="n">
         <v>1</v>
@@ -4428,18 +4521,18 @@
       <c r="DD33" s="9"/>
       <c r="DE33" s="9"/>
       <c r="DF33" s="9"/>
+      <c r="DG33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0"/>
       <c r="C34" s="16"/>
       <c r="D34" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E34" s="9" t="n">
         <v>190</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -4545,12 +4638,12 @@
       <c r="DD34" s="9"/>
       <c r="DE34" s="9"/>
       <c r="DF34" s="9"/>
+      <c r="DG34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0"/>
       <c r="C35" s="16"/>
       <c r="D35" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E35" s="9" t="n">
         <v>50</v>
@@ -4660,12 +4753,12 @@
       <c r="DD35" s="9"/>
       <c r="DE35" s="9"/>
       <c r="DF35" s="9"/>
+      <c r="DG35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0"/>
       <c r="C36" s="16"/>
       <c r="D36" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E36" s="9" t="n">
         <v>60</v>
@@ -4777,12 +4870,12 @@
       <c r="DD36" s="9"/>
       <c r="DE36" s="9"/>
       <c r="DF36" s="9"/>
+      <c r="DG36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0"/>
       <c r="C37" s="16"/>
       <c r="D37" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E37" s="9" t="n">
         <v>100</v>
@@ -4892,12 +4985,12 @@
       <c r="DD37" s="9"/>
       <c r="DE37" s="9"/>
       <c r="DF37" s="9"/>
+      <c r="DG37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0"/>
       <c r="C38" s="16"/>
       <c r="D38" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E38" s="9" t="n">
         <v>50</v>
@@ -5007,12 +5100,12 @@
       <c r="DD38" s="9"/>
       <c r="DE38" s="9"/>
       <c r="DF38" s="9"/>
+      <c r="DG38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
       <c r="C39" s="16"/>
       <c r="D39" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E39" s="9" t="n">
         <v>55</v>
@@ -5122,12 +5215,12 @@
       <c r="DD39" s="9"/>
       <c r="DE39" s="9"/>
       <c r="DF39" s="9"/>
+      <c r="DG39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
       <c r="C40" s="16"/>
       <c r="D40" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E40" s="9" t="n">
         <v>75</v>
@@ -5140,7 +5233,9 @@
       <c r="K40" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="L40" s="9"/>
+      <c r="L40" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
@@ -5239,12 +5334,12 @@
       <c r="DD40" s="9"/>
       <c r="DE40" s="9"/>
       <c r="DF40" s="9"/>
+      <c r="DG40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0"/>
       <c r="C41" s="16"/>
       <c r="D41" s="13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E41" s="9" t="n">
         <v>70</v>
@@ -5354,12 +5449,12 @@
       <c r="DD41" s="9"/>
       <c r="DE41" s="9"/>
       <c r="DF41" s="9"/>
+      <c r="DG41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0"/>
       <c r="C42" s="16"/>
       <c r="D42" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E42" s="9" t="n">
         <v>30</v>
@@ -5469,12 +5564,12 @@
       <c r="DD42" s="9"/>
       <c r="DE42" s="9"/>
       <c r="DF42" s="9"/>
+      <c r="DG42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0"/>
       <c r="C43" s="16"/>
       <c r="D43" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E43" s="9" t="n">
         <v>50</v>
@@ -5584,12 +5679,12 @@
       <c r="DD43" s="9"/>
       <c r="DE43" s="9"/>
       <c r="DF43" s="9"/>
+      <c r="DG43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0"/>
       <c r="C44" s="16"/>
       <c r="D44" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E44" s="9" t="n">
         <v>30</v>
@@ -5699,12 +5794,12 @@
       <c r="DD44" s="9"/>
       <c r="DE44" s="9"/>
       <c r="DF44" s="9"/>
+      <c r="DG44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0"/>
       <c r="C45" s="16"/>
       <c r="D45" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E45" s="9" t="n">
         <v>45</v>
@@ -5814,12 +5909,12 @@
       <c r="DD45" s="9"/>
       <c r="DE45" s="9"/>
       <c r="DF45" s="9"/>
+      <c r="DG45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0"/>
       <c r="C46" s="16"/>
       <c r="D46" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E46" s="9" t="n">
         <v>70</v>
@@ -5931,12 +6026,12 @@
       <c r="DD46" s="9"/>
       <c r="DE46" s="9"/>
       <c r="DF46" s="9"/>
+      <c r="DG46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0"/>
       <c r="C47" s="16"/>
       <c r="D47" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E47" s="9" t="n">
         <v>50</v>
@@ -6046,12 +6141,12 @@
       <c r="DD47" s="9"/>
       <c r="DE47" s="9"/>
       <c r="DF47" s="9"/>
+      <c r="DG47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0"/>
       <c r="C48" s="16"/>
       <c r="D48" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E48" s="9" t="n">
         <v>70</v>
@@ -6161,12 +6256,12 @@
       <c r="DD48" s="9"/>
       <c r="DE48" s="9"/>
       <c r="DF48" s="9"/>
+      <c r="DG48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0"/>
       <c r="C49" s="16"/>
       <c r="D49" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E49" s="9" t="n">
         <v>110</v>
@@ -6276,12 +6371,12 @@
       <c r="DD49" s="9"/>
       <c r="DE49" s="9"/>
       <c r="DF49" s="9"/>
+      <c r="DG49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0"/>
       <c r="C50" s="16"/>
       <c r="D50" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E50" s="9" t="n">
         <v>40</v>
@@ -6391,12 +6486,12 @@
       <c r="DD50" s="9"/>
       <c r="DE50" s="9"/>
       <c r="DF50" s="9"/>
+      <c r="DG50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0"/>
       <c r="C51" s="16"/>
       <c r="D51" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E51" s="9" t="n">
         <v>65</v>
@@ -6506,12 +6601,12 @@
       <c r="DD51" s="9"/>
       <c r="DE51" s="9"/>
       <c r="DF51" s="9"/>
+      <c r="DG51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0"/>
       <c r="C52" s="16"/>
       <c r="D52" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E52" s="9" t="n">
         <v>90</v>
@@ -6621,12 +6716,12 @@
       <c r="DD52" s="9"/>
       <c r="DE52" s="9"/>
       <c r="DF52" s="9"/>
+      <c r="DG52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0"/>
       <c r="C53" s="16"/>
       <c r="D53" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E53" s="9" t="n">
         <v>60</v>
@@ -6736,12 +6831,12 @@
       <c r="DD53" s="9"/>
       <c r="DE53" s="9"/>
       <c r="DF53" s="9"/>
+      <c r="DG53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0"/>
       <c r="C54" s="16"/>
       <c r="D54" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E54" s="9" t="n">
         <v>80</v>
@@ -6851,12 +6946,12 @@
       <c r="DD54" s="9"/>
       <c r="DE54" s="9"/>
       <c r="DF54" s="9"/>
+      <c r="DG54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0"/>
       <c r="C55" s="16"/>
       <c r="D55" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E55" s="9" t="n">
         <v>100</v>
@@ -6966,12 +7061,12 @@
       <c r="DD55" s="9"/>
       <c r="DE55" s="9"/>
       <c r="DF55" s="9"/>
+      <c r="DG55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0"/>
       <c r="C56" s="16"/>
       <c r="D56" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E56" s="9" t="n">
         <v>100</v>
@@ -7081,12 +7176,12 @@
       <c r="DD56" s="9"/>
       <c r="DE56" s="9"/>
       <c r="DF56" s="9"/>
+      <c r="DG56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0"/>
       <c r="C57" s="16"/>
       <c r="D57" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E57" s="9" t="n">
         <v>80</v>
@@ -7196,12 +7291,12 @@
       <c r="DD57" s="9"/>
       <c r="DE57" s="9"/>
       <c r="DF57" s="9"/>
+      <c r="DG57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0"/>
-      <c r="C58" s="17"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E58" s="9" t="n">
         <v>10</v>
@@ -7215,24 +7310,42 @@
       </c>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
+      <c r="K58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
-      <c r="O58" s="9"/>
+      <c r="O58" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="P58" s="9"/>
       <c r="Q58" s="9"/>
       <c r="R58" s="9"/>
       <c r="S58" s="9"/>
       <c r="T58" s="9"/>
-      <c r="U58" s="9"/>
+      <c r="U58" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="V58" s="9"/>
       <c r="W58" s="9"/>
-      <c r="X58" s="9"/>
-      <c r="Y58" s="9"/>
-      <c r="Z58" s="9"/>
-      <c r="AA58" s="9"/>
-      <c r="AB58" s="9"/>
+      <c r="X58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA58" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB58" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC58" s="9"/>
       <c r="AD58" s="9"/>
       <c r="AE58" s="9"/>
@@ -7315,14 +7428,14 @@
       <c r="DD58" s="9"/>
       <c r="DE58" s="9"/>
       <c r="DF58" s="9"/>
+      <c r="DG58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0"/>
       <c r="C59" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E59" s="9" t="n">
         <v>10</v>
@@ -7432,12 +7545,12 @@
       <c r="DD59" s="9"/>
       <c r="DE59" s="9"/>
       <c r="DF59" s="9"/>
+      <c r="DG59" s="9"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0"/>
       <c r="C60" s="16"/>
       <c r="D60" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E60" s="9" t="n">
         <v>15</v>
@@ -7547,12 +7660,12 @@
       <c r="DD60" s="9"/>
       <c r="DE60" s="9"/>
       <c r="DF60" s="9"/>
+      <c r="DG60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0"/>
       <c r="C61" s="16"/>
       <c r="D61" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E61" s="9" t="n">
         <v>-20</v>
@@ -7662,14 +7775,14 @@
       <c r="DD61" s="9"/>
       <c r="DE61" s="9"/>
       <c r="DF61" s="9"/>
+      <c r="DG61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0"/>
       <c r="C62" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E62" s="9" t="n">
         <v>5</v>
@@ -7679,11 +7792,19 @@
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
+      <c r="K62" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M62" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
+      <c r="O62" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="P62" s="9"/>
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
@@ -7779,12 +7900,12 @@
       <c r="DD62" s="9"/>
       <c r="DE62" s="9"/>
       <c r="DF62" s="9"/>
+      <c r="DG62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0"/>
       <c r="C63" s="16"/>
       <c r="D63" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E63" s="9" t="n">
         <v>-5</v>
@@ -7794,8 +7915,12 @@
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
+      <c r="K63" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9"/>
@@ -7803,7 +7928,9 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
-      <c r="T63" s="9"/>
+      <c r="T63" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="U63" s="9"/>
       <c r="V63" s="9"/>
       <c r="W63" s="9"/>
@@ -7894,12 +8021,12 @@
       <c r="DD63" s="9"/>
       <c r="DE63" s="9"/>
       <c r="DF63" s="9"/>
+      <c r="DG63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0"/>
       <c r="C64" s="16"/>
       <c r="D64" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E64" s="9" t="n">
         <v>10</v>
@@ -8009,12 +8136,12 @@
       <c r="DD64" s="9"/>
       <c r="DE64" s="9"/>
       <c r="DF64" s="9"/>
+      <c r="DG64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0"/>
       <c r="C65" s="16"/>
       <c r="D65" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E65" s="9" t="n">
         <v>-10</v>
@@ -8124,15 +8251,15 @@
       <c r="DD65" s="9"/>
       <c r="DE65" s="9"/>
       <c r="DF65" s="9"/>
+      <c r="DG65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0"/>
       <c r="C66" s="16"/>
       <c r="D66" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E66" s="9" t="n">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="F66" s="12"/>
       <c r="G66" s="9"/>
@@ -8141,15 +8268,21 @@
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
+      <c r="M66" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N66" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="O66" s="9"/>
       <c r="P66" s="9"/>
       <c r="Q66" s="9"/>
       <c r="R66" s="9"/>
       <c r="S66" s="9"/>
       <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
+      <c r="U66" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
       <c r="X66" s="9"/>
@@ -8239,15 +8372,15 @@
       <c r="DD66" s="9"/>
       <c r="DE66" s="9"/>
       <c r="DF66" s="9"/>
+      <c r="DG66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0"/>
       <c r="C67" s="16"/>
       <c r="D67" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E67" s="9" t="n">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="F67" s="12"/>
       <c r="G67" s="9"/>
@@ -8354,15 +8487,15 @@
       <c r="DD67" s="9"/>
       <c r="DE67" s="9"/>
       <c r="DF67" s="9"/>
+      <c r="DG67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0"/>
       <c r="C68" s="16"/>
       <c r="D68" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E68" s="9" t="n">
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="F68" s="12"/>
       <c r="G68" s="9"/>
@@ -8469,15 +8602,15 @@
       <c r="DD68" s="9"/>
       <c r="DE68" s="9"/>
       <c r="DF68" s="9"/>
+      <c r="DG68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0"/>
       <c r="C69" s="16"/>
       <c r="D69" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E69" s="9" t="n">
-        <v>15</v>
+        <v>-20</v>
       </c>
       <c r="F69" s="12"/>
       <c r="G69" s="9"/>
@@ -8584,15 +8717,15 @@
       <c r="DD69" s="9"/>
       <c r="DE69" s="9"/>
       <c r="DF69" s="9"/>
+      <c r="DG69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0"/>
       <c r="C70" s="16"/>
       <c r="D70" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E70" s="9" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F70" s="12"/>
       <c r="G70" s="9"/>
@@ -8699,15 +8832,15 @@
       <c r="DD70" s="9"/>
       <c r="DE70" s="9"/>
       <c r="DF70" s="9"/>
+      <c r="DG70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0"/>
       <c r="C71" s="16"/>
       <c r="D71" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E71" s="9" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="9"/>
@@ -8814,15 +8947,15 @@
       <c r="DD71" s="9"/>
       <c r="DE71" s="9"/>
       <c r="DF71" s="9"/>
+      <c r="DG71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0"/>
       <c r="C72" s="16"/>
       <c r="D72" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E72" s="9" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F72" s="12"/>
       <c r="G72" s="9"/>
@@ -8929,20 +9062,18 @@
       <c r="DD72" s="9"/>
       <c r="DE72" s="9"/>
       <c r="DF72" s="9"/>
+      <c r="DG72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0"/>
       <c r="C73" s="16"/>
       <c r="D73" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E73" s="9" t="n">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="F73" s="12"/>
-      <c r="G73" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
@@ -8962,8 +9093,12 @@
       <c r="X73" s="9"/>
       <c r="Y73" s="9"/>
       <c r="Z73" s="9"/>
-      <c r="AA73" s="9"/>
-      <c r="AB73" s="9"/>
+      <c r="AA73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB73" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC73" s="9"/>
       <c r="AD73" s="9"/>
       <c r="AE73" s="9"/>
@@ -9046,25 +9181,23 @@
       <c r="DD73" s="9"/>
       <c r="DE73" s="9"/>
       <c r="DF73" s="9"/>
+      <c r="DG73" s="9"/>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0"/>
-      <c r="C74" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D74" s="11" t="s">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="16"/>
+      <c r="D74" s="13" t="s">
         <v>121</v>
       </c>
       <c r="E74" s="9" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="F74" s="12"/>
-      <c r="G74" s="9"/>
+      <c r="G74" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
-      <c r="J74" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="J74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
@@ -9081,8 +9214,12 @@
       <c r="X74" s="9"/>
       <c r="Y74" s="9"/>
       <c r="Z74" s="9"/>
-      <c r="AA74" s="9"/>
-      <c r="AB74" s="9"/>
+      <c r="AA74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB74" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="AC74" s="9"/>
       <c r="AD74" s="9"/>
       <c r="AE74" s="9"/>
@@ -9165,34 +9302,30 @@
       <c r="DD74" s="9"/>
       <c r="DE74" s="9"/>
       <c r="DF74" s="9"/>
+      <c r="DG74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0"/>
       <c r="C75" s="16"/>
       <c r="D75" s="13" t="s">
         <v>122</v>
       </c>
       <c r="E75" s="9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F75" s="12"/>
-      <c r="G75" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="9"/>
+      <c r="N75" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O75" s="9" t="n">
+        <v>4</v>
+      </c>
       <c r="P75" s="9"/>
       <c r="Q75" s="9"/>
       <c r="R75" s="9"/>
@@ -9288,20 +9421,20 @@
       <c r="DD75" s="9"/>
       <c r="DE75" s="9"/>
       <c r="DF75" s="9"/>
+      <c r="DG75" s="9"/>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="14" t="s">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C76" s="16" t="s">
         <v>123</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="E76" s="9" t="n">
         <v>10</v>
       </c>
       <c r="F76" s="12"/>
-      <c r="G76" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="G76" s="9"/>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9" t="n">
@@ -9311,1314 +9444,1574 @@
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
+      <c r="O76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="9"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="9"/>
+      <c r="V76" s="9"/>
+      <c r="W76" s="9"/>
+      <c r="X76" s="9"/>
+      <c r="Y76" s="9"/>
+      <c r="Z76" s="9"/>
+      <c r="AA76" s="9"/>
+      <c r="AB76" s="9"/>
+      <c r="AC76" s="9"/>
+      <c r="AD76" s="9"/>
+      <c r="AE76" s="9"/>
+      <c r="AF76" s="9"/>
+      <c r="AG76" s="9"/>
+      <c r="AH76" s="9"/>
+      <c r="AI76" s="9"/>
+      <c r="AJ76" s="9"/>
+      <c r="AK76" s="9"/>
+      <c r="AL76" s="9"/>
+      <c r="AM76" s="9"/>
+      <c r="AN76" s="9"/>
+      <c r="AO76" s="9"/>
+      <c r="AP76" s="9"/>
+      <c r="AQ76" s="9"/>
+      <c r="AR76" s="9"/>
+      <c r="AS76" s="9"/>
+      <c r="AT76" s="9"/>
+      <c r="AU76" s="9"/>
+      <c r="AV76" s="9"/>
+      <c r="AW76" s="9"/>
+      <c r="AX76" s="9"/>
+      <c r="AY76" s="9"/>
+      <c r="AZ76" s="9"/>
+      <c r="BA76" s="9"/>
+      <c r="BB76" s="9"/>
+      <c r="BC76" s="9"/>
+      <c r="BD76" s="9"/>
+      <c r="BE76" s="9"/>
+      <c r="BF76" s="9"/>
+      <c r="BG76" s="9"/>
+      <c r="BH76" s="9"/>
+      <c r="BI76" s="9"/>
+      <c r="BJ76" s="9"/>
+      <c r="BK76" s="9"/>
+      <c r="BL76" s="9"/>
+      <c r="BM76" s="9"/>
+      <c r="BN76" s="9"/>
+      <c r="BO76" s="9"/>
+      <c r="BP76" s="9"/>
+      <c r="BQ76" s="9"/>
+      <c r="BR76" s="9"/>
+      <c r="BS76" s="9"/>
+      <c r="BT76" s="9"/>
+      <c r="BU76" s="9"/>
+      <c r="BV76" s="9"/>
+      <c r="BW76" s="9"/>
+      <c r="BX76" s="9"/>
+      <c r="BY76" s="9"/>
+      <c r="BZ76" s="9"/>
+      <c r="CA76" s="9"/>
+      <c r="CB76" s="9"/>
+      <c r="CC76" s="9"/>
+      <c r="CD76" s="9"/>
+      <c r="CE76" s="9"/>
+      <c r="CF76" s="9"/>
+      <c r="CG76" s="9"/>
+      <c r="CH76" s="9"/>
+      <c r="CI76" s="9"/>
+      <c r="CJ76" s="9"/>
+      <c r="CK76" s="9"/>
+      <c r="CL76" s="9"/>
+      <c r="CM76" s="9"/>
+      <c r="CN76" s="9"/>
+      <c r="CO76" s="9"/>
+      <c r="CP76" s="9"/>
+      <c r="CQ76" s="9"/>
+      <c r="CR76" s="9"/>
+      <c r="CS76" s="9"/>
+      <c r="CT76" s="9"/>
+      <c r="CU76" s="9"/>
+      <c r="CV76" s="9"/>
+      <c r="CW76" s="9"/>
+      <c r="CX76" s="9"/>
+      <c r="CY76" s="9"/>
+      <c r="CZ76" s="9"/>
+      <c r="DA76" s="9"/>
+      <c r="DB76" s="9"/>
+      <c r="DC76" s="9"/>
+      <c r="DD76" s="9"/>
+      <c r="DE76" s="9"/>
+      <c r="DF76" s="9"/>
+      <c r="DG76" s="9"/>
     </row>
-    <row r="77" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0"/>
-      <c r="E77" s="9"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="16"/>
+      <c r="D77" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E77" s="9" t="n">
+        <v>10</v>
+      </c>
       <c r="F77" s="12"/>
-      <c r="J77" s="1"/>
+      <c r="G77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="9"/>
+      <c r="R77" s="9"/>
+      <c r="S77" s="9"/>
+      <c r="T77" s="9"/>
+      <c r="U77" s="9"/>
+      <c r="V77" s="9"/>
+      <c r="W77" s="9"/>
+      <c r="X77" s="9"/>
+      <c r="Y77" s="9"/>
+      <c r="Z77" s="9"/>
+      <c r="AA77" s="9"/>
+      <c r="AB77" s="9"/>
+      <c r="AC77" s="9"/>
+      <c r="AD77" s="9"/>
+      <c r="AE77" s="9"/>
+      <c r="AF77" s="9"/>
+      <c r="AG77" s="9"/>
+      <c r="AH77" s="9"/>
+      <c r="AI77" s="9"/>
+      <c r="AJ77" s="9"/>
+      <c r="AK77" s="9"/>
+      <c r="AL77" s="9"/>
+      <c r="AM77" s="9"/>
+      <c r="AN77" s="9"/>
+      <c r="AO77" s="9"/>
+      <c r="AP77" s="9"/>
+      <c r="AQ77" s="9"/>
+      <c r="AR77" s="9"/>
+      <c r="AS77" s="9"/>
+      <c r="AT77" s="9"/>
+      <c r="AU77" s="9"/>
+      <c r="AV77" s="9"/>
+      <c r="AW77" s="9"/>
+      <c r="AX77" s="9"/>
+      <c r="AY77" s="9"/>
+      <c r="AZ77" s="9"/>
+      <c r="BA77" s="9"/>
+      <c r="BB77" s="9"/>
+      <c r="BC77" s="9"/>
+      <c r="BD77" s="9"/>
+      <c r="BE77" s="9"/>
+      <c r="BF77" s="9"/>
+      <c r="BG77" s="9"/>
+      <c r="BH77" s="9"/>
+      <c r="BI77" s="9"/>
+      <c r="BJ77" s="9"/>
+      <c r="BK77" s="9"/>
+      <c r="BL77" s="9"/>
+      <c r="BM77" s="9"/>
+      <c r="BN77" s="9"/>
+      <c r="BO77" s="9"/>
+      <c r="BP77" s="9"/>
+      <c r="BQ77" s="9"/>
+      <c r="BR77" s="9"/>
+      <c r="BS77" s="9"/>
+      <c r="BT77" s="9"/>
+      <c r="BU77" s="9"/>
+      <c r="BV77" s="9"/>
+      <c r="BW77" s="9"/>
+      <c r="BX77" s="9"/>
+      <c r="BY77" s="9"/>
+      <c r="BZ77" s="9"/>
+      <c r="CA77" s="9"/>
+      <c r="CB77" s="9"/>
+      <c r="CC77" s="9"/>
+      <c r="CD77" s="9"/>
+      <c r="CE77" s="9"/>
+      <c r="CF77" s="9"/>
+      <c r="CG77" s="9"/>
+      <c r="CH77" s="9"/>
+      <c r="CI77" s="9"/>
+      <c r="CJ77" s="9"/>
+      <c r="CK77" s="9"/>
+      <c r="CL77" s="9"/>
+      <c r="CM77" s="9"/>
+      <c r="CN77" s="9"/>
+      <c r="CO77" s="9"/>
+      <c r="CP77" s="9"/>
+      <c r="CQ77" s="9"/>
+      <c r="CR77" s="9"/>
+      <c r="CS77" s="9"/>
+      <c r="CT77" s="9"/>
+      <c r="CU77" s="9"/>
+      <c r="CV77" s="9"/>
+      <c r="CW77" s="9"/>
+      <c r="CX77" s="9"/>
+      <c r="CY77" s="9"/>
+      <c r="CZ77" s="9"/>
+      <c r="DA77" s="9"/>
+      <c r="DB77" s="9"/>
+      <c r="DC77" s="9"/>
+      <c r="DD77" s="9"/>
+      <c r="DE77" s="9"/>
+      <c r="DF77" s="9"/>
+      <c r="DG77" s="9"/>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="21" t="str">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="16"/>
+      <c r="D78" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E78" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F78" s="12"/>
+      <c r="G78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+    </row>
+    <row r="79" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E79" s="9"/>
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C80" s="17"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="20" t="str">
         <f aca="false">G4</f>
         <v>Leopard 2A6</v>
       </c>
-      <c r="H78" s="21" t="str">
+      <c r="H80" s="20" t="str">
         <f aca="false">H4</f>
         <v>PzH 2000</v>
       </c>
-      <c r="I78" s="21" t="str">
+      <c r="I80" s="20" t="str">
         <f aca="false">I4</f>
         <v>MARS II</v>
       </c>
-      <c r="J78" s="21" t="str">
+      <c r="J80" s="20" t="str">
         <f aca="false">J4</f>
         <v>Eurocopter</v>
       </c>
-      <c r="K78" s="21" t="str">
+      <c r="K80" s="20" t="str">
         <f aca="false">K4</f>
+        <v>M113 mortar</v>
+      </c>
+      <c r="L80" s="20" t="str">
+        <f aca="false">L4</f>
         <v>Wiesel I Mörser 120mm </v>
       </c>
-      <c r="L78" s="21" t="str">
-        <f aca="false">L4</f>
+      <c r="M80" s="20" t="str">
+        <f aca="false">M4</f>
         <v>M113 Feuerleitpanzer </v>
       </c>
-      <c r="M78" s="21" t="str">
-        <f aca="false">M4</f>
+      <c r="N80" s="20" t="str">
+        <f aca="false">N4</f>
         <v>Joint Fire Support Team Fennek 1A4 </v>
       </c>
-      <c r="N78" s="21" t="str">
-        <f aca="false">N4</f>
+      <c r="O80" s="20" t="str">
+        <f aca="false">O4</f>
         <v>Störpanzer Hummel </v>
       </c>
-      <c r="O78" s="21" t="str">
-        <f aca="false">O4</f>
+      <c r="P80" s="20" t="str">
+        <f aca="false">P4</f>
         <v>Eagle IV APC </v>
       </c>
-      <c r="P78" s="21" t="str">
-        <f aca="false">P4</f>
+      <c r="Q80" s="20" t="str">
+        <f aca="false">Q4</f>
         <v>Eagle V APC </v>
       </c>
-      <c r="Q78" s="21" t="str">
-        <f aca="false">Q4</f>
+      <c r="R80" s="20" t="str">
+        <f aca="false">R4</f>
         <v>Enok 6.1 LAPV </v>
       </c>
-      <c r="R78" s="21" t="str">
-        <f aca="false">R4</f>
+      <c r="S80" s="20" t="str">
+        <f aca="false">S4</f>
         <v>Duro 3 Yak </v>
       </c>
-      <c r="S78" s="21" t="str">
-        <f aca="false">S4</f>
+      <c r="T80" s="20" t="str">
+        <f aca="false">T4</f>
         <v>ESK Mungo </v>
       </c>
-      <c r="T78" s="21" t="str">
-        <f aca="false">T4</f>
+      <c r="U80" s="20" t="str">
+        <f aca="false">U4</f>
         <v>LGS Fennek </v>
       </c>
-      <c r="U78" s="21" t="str">
-        <f aca="false">U4</f>
+      <c r="V80" s="20" t="str">
+        <f aca="false">V4</f>
         <v>ATF Dingo 1 </v>
       </c>
-      <c r="V78" s="21" t="str">
-        <f aca="false">V4</f>
+      <c r="W80" s="20" t="str">
+        <f aca="false">W4</f>
         <v>ATF Dingo 2 </v>
       </c>
-      <c r="W78" s="21" t="str">
-        <f aca="false">W4</f>
+      <c r="X80" s="20" t="str">
+        <f aca="false">X4</f>
         <v>M113 </v>
       </c>
-      <c r="X78" s="21" t="str">
-        <f aca="false">X4</f>
+      <c r="Y80" s="20" t="str">
+        <f aca="false">Y4</f>
         <v>TPz Fuchs 1A4/5 </v>
       </c>
-      <c r="Y78" s="21" t="str">
-        <f aca="false">Y4</f>
+      <c r="Z80" s="20" t="str">
+        <f aca="false">Z4</f>
         <v>GTK Boxer </v>
       </c>
-      <c r="Z78" s="21" t="str">
-        <f aca="false">Z4</f>
+      <c r="AA80" s="20" t="str">
+        <f aca="false">AA4</f>
         <v>SPz 1A3 Marder </v>
       </c>
-      <c r="AA78" s="21" t="str">
-        <f aca="false">AA4</f>
+      <c r="AB80" s="20" t="str">
+        <f aca="false">AB4</f>
         <v>SPz Puma </v>
       </c>
-      <c r="AB78" s="21" t="str">
-        <f aca="false">AB4</f>
+      <c r="AC80" s="20" t="str">
+        <f aca="false">AC4</f>
         <v>AGF Serval LIV (SO) </v>
       </c>
-      <c r="AC78" s="21" t="str">
-        <f aca="false">AC4</f>
+      <c r="AD80" s="20" t="str">
+        <f aca="false">AD4</f>
         <v>Wiesel I </v>
       </c>
-      <c r="AD78" s="21" t="str">
-        <f aca="false">AD4</f>
+      <c r="AE80" s="20" t="str">
+        <f aca="false">AE4</f>
         <v>Wiesel I TOW </v>
       </c>
-      <c r="AE78" s="21" t="str">
-        <f aca="false">AE4</f>
+      <c r="AF80" s="20" t="str">
+        <f aca="false">AF4</f>
         <v>Wiesel I A3 MK </v>
       </c>
-      <c r="AF78" s="21" t="str">
-        <f aca="false">AF4</f>
+      <c r="AG80" s="20" t="str">
+        <f aca="false">AG4</f>
         <v>M113 Transport </v>
       </c>
-      <c r="AG78" s="21" t="str">
-        <f aca="false">AG4</f>
+      <c r="AH80" s="20" t="str">
+        <f aca="false">AH4</f>
         <v>TPz Fuchs 1A4/5 Transport </v>
       </c>
-      <c r="AH78" s="21" t="str">
-        <f aca="false">AH4</f>
+      <c r="AI80" s="20" t="str">
+        <f aca="false">AI4</f>
         <v>GTK Boxer Tranport </v>
       </c>
-      <c r="AI78" s="21" t="str">
-        <f aca="false">AI4</f>
+      <c r="AJ80" s="20" t="str">
+        <f aca="false">AJ4</f>
         <v>MAN gl Transport </v>
       </c>
-      <c r="AJ78" s="21" t="str">
-        <f aca="false">AJ4</f>
+      <c r="AK80" s="20" t="str">
+        <f aca="false">AK4</f>
         <v>Unimog Transport </v>
       </c>
-      <c r="AK78" s="21" t="str">
-        <f aca="false">AK4</f>
+      <c r="AL80" s="20" t="str">
+        <f aca="false">AL4</f>
         <v>Wolf G5 Jeep Transport </v>
       </c>
-      <c r="AL78" s="21" t="n">
-        <f aca="false">AL4</f>
-        <v>0</v>
-      </c>
-      <c r="AM78" s="21" t="n">
+      <c r="AM80" s="20" t="n">
         <f aca="false">AM4</f>
         <v>0</v>
       </c>
-      <c r="AN78" s="21" t="n">
+      <c r="AN80" s="20" t="n">
         <f aca="false">AN4</f>
         <v>0</v>
       </c>
-      <c r="AO78" s="21" t="n">
+      <c r="AO80" s="20" t="n">
         <f aca="false">AO4</f>
         <v>0</v>
       </c>
-      <c r="AP78" s="21" t="n">
+      <c r="AP80" s="20" t="n">
         <f aca="false">AP4</f>
         <v>0</v>
       </c>
-      <c r="AQ78" s="21" t="n">
+      <c r="AQ80" s="20" t="n">
         <f aca="false">AQ4</f>
         <v>0</v>
       </c>
-      <c r="AR78" s="21" t="n">
+      <c r="AR80" s="20" t="n">
         <f aca="false">AR4</f>
         <v>0</v>
       </c>
-      <c r="AS78" s="21" t="n">
+      <c r="AS80" s="20" t="n">
         <f aca="false">AS4</f>
         <v>0</v>
       </c>
-      <c r="AT78" s="21" t="n">
+      <c r="AT80" s="20" t="n">
         <f aca="false">AT4</f>
         <v>0</v>
       </c>
-      <c r="AU78" s="21" t="n">
+      <c r="AU80" s="20" t="n">
         <f aca="false">AU4</f>
         <v>0</v>
       </c>
-      <c r="AV78" s="21" t="n">
+      <c r="AV80" s="20" t="n">
         <f aca="false">AV4</f>
         <v>0</v>
       </c>
-      <c r="AW78" s="21" t="n">
+      <c r="AW80" s="20" t="n">
         <f aca="false">AW4</f>
         <v>0</v>
       </c>
-      <c r="AX78" s="21" t="n">
+      <c r="AX80" s="20" t="n">
         <f aca="false">AX4</f>
         <v>0</v>
       </c>
-      <c r="AY78" s="21" t="n">
+      <c r="AY80" s="20" t="n">
         <f aca="false">AY4</f>
         <v>0</v>
       </c>
-      <c r="AZ78" s="21" t="n">
+      <c r="AZ80" s="20" t="n">
         <f aca="false">AZ4</f>
         <v>0</v>
       </c>
-      <c r="BA78" s="21" t="n">
+      <c r="BA80" s="20" t="n">
         <f aca="false">BA4</f>
         <v>0</v>
       </c>
-      <c r="BB78" s="21" t="n">
+      <c r="BB80" s="20" t="n">
         <f aca="false">BB4</f>
         <v>0</v>
       </c>
-      <c r="BC78" s="21" t="n">
+      <c r="BC80" s="20" t="n">
         <f aca="false">BC4</f>
         <v>0</v>
       </c>
-      <c r="BD78" s="21" t="n">
+      <c r="BD80" s="20" t="n">
         <f aca="false">BD4</f>
         <v>0</v>
       </c>
-      <c r="BE78" s="21" t="n">
+      <c r="BE80" s="20" t="n">
         <f aca="false">BE4</f>
         <v>0</v>
       </c>
-      <c r="BF78" s="21" t="n">
+      <c r="BF80" s="20" t="n">
         <f aca="false">BF4</f>
         <v>0</v>
       </c>
-      <c r="BG78" s="21" t="n">
+      <c r="BG80" s="20" t="n">
         <f aca="false">BG4</f>
         <v>0</v>
       </c>
-      <c r="BH78" s="21" t="n">
+      <c r="BH80" s="20" t="n">
         <f aca="false">BH4</f>
         <v>0</v>
       </c>
-      <c r="BI78" s="21" t="n">
+      <c r="BI80" s="20" t="n">
         <f aca="false">BI4</f>
         <v>0</v>
       </c>
-      <c r="BJ78" s="21" t="n">
+      <c r="BJ80" s="20" t="n">
         <f aca="false">BJ4</f>
         <v>0</v>
       </c>
-      <c r="BK78" s="21" t="n">
+      <c r="BK80" s="20" t="n">
         <f aca="false">BK4</f>
         <v>0</v>
       </c>
-      <c r="BL78" s="21" t="n">
+      <c r="BL80" s="20" t="n">
         <f aca="false">BL4</f>
         <v>0</v>
       </c>
-      <c r="BM78" s="21" t="n">
+      <c r="BM80" s="20" t="n">
         <f aca="false">BM4</f>
         <v>0</v>
       </c>
-      <c r="BN78" s="21" t="n">
+      <c r="BN80" s="20" t="n">
         <f aca="false">BN4</f>
         <v>0</v>
       </c>
-      <c r="BO78" s="21" t="n">
+      <c r="BO80" s="20" t="n">
         <f aca="false">BO4</f>
         <v>0</v>
       </c>
-      <c r="BP78" s="21" t="n">
+      <c r="BP80" s="20" t="n">
         <f aca="false">BP4</f>
         <v>0</v>
       </c>
-      <c r="BQ78" s="21" t="n">
+      <c r="BQ80" s="20" t="n">
         <f aca="false">BQ4</f>
         <v>0</v>
       </c>
-      <c r="BR78" s="21" t="n">
+      <c r="BR80" s="20" t="n">
         <f aca="false">BR4</f>
         <v>0</v>
       </c>
-      <c r="BS78" s="21" t="n">
+      <c r="BS80" s="20" t="n">
         <f aca="false">BS4</f>
         <v>0</v>
       </c>
-      <c r="BT78" s="21" t="n">
+      <c r="BT80" s="20" t="n">
         <f aca="false">BT4</f>
         <v>0</v>
       </c>
-      <c r="BU78" s="21" t="n">
+      <c r="BU80" s="20" t="n">
         <f aca="false">BU4</f>
         <v>0</v>
       </c>
-      <c r="BV78" s="21" t="n">
+      <c r="BV80" s="20" t="n">
         <f aca="false">BV4</f>
         <v>0</v>
       </c>
-      <c r="BW78" s="21" t="n">
+      <c r="BW80" s="20" t="n">
         <f aca="false">BW4</f>
         <v>0</v>
       </c>
-      <c r="BX78" s="21" t="n">
+      <c r="BX80" s="20" t="n">
         <f aca="false">BX4</f>
         <v>0</v>
       </c>
-      <c r="BY78" s="21" t="n">
+      <c r="BY80" s="20" t="n">
         <f aca="false">BY4</f>
         <v>0</v>
       </c>
-      <c r="BZ78" s="21" t="n">
+      <c r="BZ80" s="20" t="n">
         <f aca="false">BZ4</f>
         <v>0</v>
       </c>
-      <c r="CA78" s="21" t="n">
+      <c r="CA80" s="20" t="n">
         <f aca="false">CA4</f>
         <v>0</v>
       </c>
-      <c r="CB78" s="21" t="n">
+      <c r="CB80" s="20" t="n">
         <f aca="false">CB4</f>
         <v>0</v>
       </c>
-      <c r="CC78" s="21" t="n">
+      <c r="CC80" s="20" t="n">
         <f aca="false">CC4</f>
         <v>0</v>
       </c>
-      <c r="CD78" s="21" t="n">
+      <c r="CD80" s="20" t="n">
         <f aca="false">CD4</f>
         <v>0</v>
       </c>
-      <c r="CE78" s="21" t="n">
+      <c r="CE80" s="20" t="n">
         <f aca="false">CE4</f>
         <v>0</v>
       </c>
-      <c r="CF78" s="21" t="n">
+      <c r="CF80" s="20" t="n">
         <f aca="false">CF4</f>
         <v>0</v>
       </c>
-      <c r="CG78" s="21" t="n">
+      <c r="CG80" s="20" t="n">
         <f aca="false">CG4</f>
         <v>0</v>
       </c>
+      <c r="CH80" s="20" t="n">
+        <f aca="false">CH4</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0"/>
-      <c r="C79" s="16" t="s">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C81" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E81" s="9" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G81" s="9" t="n">
+        <f aca="false">ROUNDUP(G82*E81,0)</f>
+        <v>230</v>
+      </c>
+      <c r="H81" s="9" t="n">
+        <f aca="false">ROUNDUP(H82*$E81,0)</f>
+        <v>117</v>
+      </c>
+      <c r="I81" s="9" t="n">
+        <f aca="false">ROUNDUP(I82*$E81,0)</f>
+        <v>117</v>
+      </c>
+      <c r="J81" s="9" t="n">
+        <f aca="false">ROUNDUP(J82*$E81,0)</f>
+        <v>144</v>
+      </c>
+      <c r="K81" s="9" t="n">
+        <f aca="false">ROUNDUP(K82*$E81,0)</f>
+        <v>122</v>
+      </c>
+      <c r="L81" s="9" t="n">
+        <f aca="false">ROUNDUP(L82*$E81,0)</f>
+        <v>122</v>
+      </c>
+      <c r="M81" s="9" t="n">
+        <f aca="false">ROUNDUP(M82*$E81,0)</f>
+        <v>59</v>
+      </c>
+      <c r="N81" s="9" t="n">
+        <f aca="false">ROUNDUP(N82*$E81,0)</f>
+        <v>72</v>
+      </c>
+      <c r="O81" s="9" t="n">
+        <f aca="false">ROUNDUP(O82*$E81,0)</f>
+        <v>86</v>
+      </c>
+      <c r="P81" s="9" t="n">
+        <f aca="false">ROUNDUP(P82*$E81,0)</f>
+        <v>49</v>
+      </c>
+      <c r="Q81" s="9" t="n">
+        <f aca="false">ROUNDUP(Q82*$E81,0)</f>
+        <v>49</v>
+      </c>
+      <c r="R81" s="9" t="n">
+        <f aca="false">ROUNDUP(R82*$E81,0)</f>
+        <v>53</v>
+      </c>
+      <c r="S81" s="9" t="n">
+        <f aca="false">ROUNDUP(S82*$E81,0)</f>
+        <v>74</v>
+      </c>
+      <c r="T81" s="9" t="n">
+        <f aca="false">ROUNDUP(T82*$E81,0)</f>
+        <v>55</v>
+      </c>
+      <c r="U81" s="9" t="n">
+        <f aca="false">ROUNDUP(U82*$E81,0)</f>
+        <v>67</v>
+      </c>
+      <c r="V81" s="9" t="n">
+        <f aca="false">ROUNDUP(V82*$E81,0)</f>
+        <v>49</v>
+      </c>
+      <c r="W81" s="9" t="n">
+        <f aca="false">ROUNDUP(W82*$E81,0)</f>
+        <v>54</v>
+      </c>
+      <c r="X81" s="9" t="n">
+        <f aca="false">ROUNDUP(X82*$E81,0)</f>
+        <v>74</v>
+      </c>
+      <c r="Y81" s="9" t="n">
+        <f aca="false">ROUNDUP(Y82*$E81,0)</f>
+        <v>69</v>
+      </c>
+      <c r="Z81" s="9" t="n">
+        <f aca="false">ROUNDUP(Z82*$E81,0)</f>
+        <v>67</v>
+      </c>
+      <c r="AA81" s="9" t="n">
+        <f aca="false">ROUNDUP(AA82*$E81,0)</f>
+        <v>101</v>
+      </c>
+      <c r="AB81" s="9" t="n">
+        <f aca="false">ROUNDUP(AB82*$E81,0)</f>
+        <v>128</v>
+      </c>
+      <c r="AC81" s="9" t="n">
+        <f aca="false">ROUNDUP(AC82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD81" s="9" t="n">
+        <f aca="false">ROUNDUP(AD82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE81" s="9" t="n">
+        <f aca="false">ROUNDUP(AE82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF81" s="9" t="n">
+        <f aca="false">ROUNDUP(AF82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG81" s="9" t="n">
+        <f aca="false">ROUNDUP(AG82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH81" s="9" t="n">
+        <f aca="false">ROUNDUP(AH82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI81" s="9" t="n">
+        <f aca="false">ROUNDUP(AI82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ81" s="9" t="n">
+        <f aca="false">ROUNDUP(AJ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AK81" s="9" t="n">
+        <f aca="false">ROUNDUP(AK82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AL81" s="9" t="n">
+        <f aca="false">ROUNDUP(AL82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AM81" s="9" t="n">
+        <f aca="false">ROUNDUP(AM82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN81" s="9" t="n">
+        <f aca="false">ROUNDUP(AN82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO81" s="9" t="n">
+        <f aca="false">ROUNDUP(AO82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP81" s="9" t="n">
+        <f aca="false">ROUNDUP(AP82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ81" s="9" t="n">
+        <f aca="false">ROUNDUP(AQ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR81" s="9" t="n">
+        <f aca="false">ROUNDUP(AR82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS81" s="9" t="n">
+        <f aca="false">ROUNDUP(AS82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT81" s="9" t="n">
+        <f aca="false">ROUNDUP(AT82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AU81" s="9" t="n">
+        <f aca="false">ROUNDUP(AU82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV81" s="9" t="n">
+        <f aca="false">ROUNDUP(AV82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AW81" s="9" t="n">
+        <f aca="false">ROUNDUP(AW82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX81" s="9" t="n">
+        <f aca="false">ROUNDUP(AX82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AY81" s="9" t="n">
+        <f aca="false">ROUNDUP(AY82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ81" s="9" t="n">
+        <f aca="false">ROUNDUP(AZ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BA81" s="9" t="n">
+        <f aca="false">ROUNDUP(BA82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB81" s="9" t="n">
+        <f aca="false">ROUNDUP(BB82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BC81" s="9" t="n">
+        <f aca="false">ROUNDUP(BC82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BD81" s="9" t="n">
+        <f aca="false">ROUNDUP(BD82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BE81" s="9" t="n">
+        <f aca="false">ROUNDUP(BE82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF81" s="9" t="n">
+        <f aca="false">ROUNDUP(BF82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BG81" s="9" t="n">
+        <f aca="false">ROUNDUP(BG82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BH81" s="9" t="n">
+        <f aca="false">ROUNDUP(BH82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BI81" s="9" t="n">
+        <f aca="false">ROUNDUP(BI82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ81" s="9" t="n">
+        <f aca="false">ROUNDUP(BJ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BK81" s="9" t="n">
+        <f aca="false">ROUNDUP(BK82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BL81" s="9" t="n">
+        <f aca="false">ROUNDUP(BL82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BM81" s="9" t="n">
+        <f aca="false">ROUNDUP(BM82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BN81" s="9" t="n">
+        <f aca="false">ROUNDUP(BN82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BO81" s="9" t="n">
+        <f aca="false">ROUNDUP(BO82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BP81" s="9" t="n">
+        <f aca="false">ROUNDUP(BP82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ81" s="9" t="n">
+        <f aca="false">ROUNDUP(BQ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR81" s="9" t="n">
+        <f aca="false">ROUNDUP(BR82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BS81" s="9" t="n">
+        <f aca="false">ROUNDUP(BS82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BT81" s="9" t="n">
+        <f aca="false">ROUNDUP(BT82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BU81" s="9" t="n">
+        <f aca="false">ROUNDUP(BU82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BV81" s="9" t="n">
+        <f aca="false">ROUNDUP(BV82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BW81" s="9" t="n">
+        <f aca="false">ROUNDUP(BW82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BX81" s="9" t="n">
+        <f aca="false">ROUNDUP(BX82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BY81" s="9" t="n">
+        <f aca="false">ROUNDUP(BY82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ81" s="9" t="n">
+        <f aca="false">ROUNDUP(BZ82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CA81" s="9" t="n">
+        <f aca="false">ROUNDUP(CA82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CB81" s="9" t="n">
+        <f aca="false">ROUNDUP(CB82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CC81" s="9" t="n">
+        <f aca="false">ROUNDUP(CC82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CD81" s="9" t="n">
+        <f aca="false">ROUNDUP(CD82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CE81" s="9" t="n">
+        <f aca="false">ROUNDUP(CE82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CF81" s="9" t="n">
+        <f aca="false">ROUNDUP(CF82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CG81" s="9" t="n">
+        <f aca="false">ROUNDUP(CG82*$E81,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CH81" s="9" t="n">
+        <f aca="false">ROUNDUP(CH82*$E81,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="16"/>
+      <c r="D82" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(G6:G80, E6:E80)</f>
+        <v>255</v>
+      </c>
+      <c r="H82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(H6:H80, $E6:$E80)</f>
+        <v>130</v>
+      </c>
+      <c r="I82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(I6:I80, $E6:$E80)</f>
+        <v>130</v>
+      </c>
+      <c r="J82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(J6:J80, $E6:$E80)</f>
+        <v>160</v>
+      </c>
+      <c r="K82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(K6:K80, $E6:$E80)</f>
+        <v>135</v>
+      </c>
+      <c r="L82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(L6:L80, $E6:$E80)</f>
+        <v>135</v>
+      </c>
+      <c r="M82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(M6:M80, $E6:$E80)</f>
+        <v>65</v>
+      </c>
+      <c r="N82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(N6:N80, $E6:$E80)</f>
+        <v>80</v>
+      </c>
+      <c r="O82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(O6:O80, $E6:$E80)</f>
+        <v>95</v>
+      </c>
+      <c r="P82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(P6:P80, $E6:$E80)</f>
+        <v>54</v>
+      </c>
+      <c r="Q82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(Q6:Q80, $E6:$E80)</f>
+        <v>54</v>
+      </c>
+      <c r="R82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(R6:R80, $E6:$E80)</f>
+        <v>58</v>
+      </c>
+      <c r="S82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(S6:S80, $E6:$E80)</f>
+        <v>82</v>
+      </c>
+      <c r="T82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(T6:T80, $E6:$E80)</f>
+        <v>61</v>
+      </c>
+      <c r="U82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(U6:U80, $E6:$E80)</f>
+        <v>74</v>
+      </c>
+      <c r="V82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(V6:V80, $E6:$E80)</f>
+        <v>54</v>
+      </c>
+      <c r="W82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(W6:W80, $E6:$E80)</f>
+        <v>60</v>
+      </c>
+      <c r="X82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(X6:X80, $E6:$E80)</f>
+        <v>82</v>
+      </c>
+      <c r="Y82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(Y6:Y80, $E6:$E80)</f>
+        <v>76</v>
+      </c>
+      <c r="Z82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(Z6:Z80, $E6:$E80)</f>
+        <v>74</v>
+      </c>
+      <c r="AA82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AA6:AA80, $E6:$E80)</f>
+        <v>112</v>
+      </c>
+      <c r="AB82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AB6:AB80, $E6:$E80)</f>
+        <v>142</v>
+      </c>
+      <c r="AC82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AC6:AC80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AD82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AD6:AD80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AE82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AE6:AE80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AF82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AF6:AF80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AG82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AG6:AG80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AH82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AH6:AH80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AI82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AI6:AI80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AJ6:AJ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AK82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AK6:AK80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AL82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AL6:AL80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AM82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AM6:AM80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AN82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AN6:AN80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AO82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AO6:AO80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AP82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AP6:AP80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AQ6:AQ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AR82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AR6:AR80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AS82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AS6:AS80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AT82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AT6:AT80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AU82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AU6:AU80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AV82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AV6:AV80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AW82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AW6:AW80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AX82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AX6:AX80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AY82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AY6:AY80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(AZ6:AZ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BA82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BA6:BA80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BB82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BB6:BB80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BC82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BC6:BC80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BD82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BD6:BD80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BE82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BE6:BE80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BF82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BF6:BF80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BG82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BG6:BG80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BH82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BH6:BH80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BI82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BI6:BI80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BJ6:BJ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BK82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BK6:BK80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BL82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BL6:BL80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BM82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BM6:BM80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BN82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BN6:BN80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BO82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BO6:BO80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BP82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BP6:BP80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BQ6:BQ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BR82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BR6:BR80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BS82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BS6:BS80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BT82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BT6:BT80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BU82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BU6:BU80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BV82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BV6:BV80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BW82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BW6:BW80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BX82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BX6:BX80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BY82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BY6:BY80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(BZ6:BZ80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CA82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CA6:CA80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CB82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CB6:CB80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CC82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CC6:CC80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CD82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CD6:CD80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CE82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CE6:CE80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CF82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CF6:CF80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CG82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CG6:CG80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+      <c r="CH82" s="9" t="n">
+        <f aca="false">SUMPRODUCT(CH6:CH80, $E6:$E80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="16"/>
+      <c r="D83" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E83" s="9" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G83" s="9" t="n">
+        <f aca="false">ROUNDUP(G82*E83,0)</f>
+        <v>281</v>
+      </c>
+      <c r="H83" s="9" t="n">
+        <f aca="false">ROUNDUP(H82*$E83,0)</f>
+        <v>143</v>
+      </c>
+      <c r="I83" s="9" t="n">
+        <f aca="false">ROUNDUP(I82*$E83,0)</f>
+        <v>143</v>
+      </c>
+      <c r="J83" s="9" t="n">
+        <f aca="false">ROUNDUP(J82*$E83,0)</f>
+        <v>176</v>
+      </c>
+      <c r="K83" s="9" t="n">
+        <f aca="false">ROUNDUP(K82*$E83,0)</f>
+        <v>149</v>
+      </c>
+      <c r="L83" s="9" t="n">
+        <f aca="false">ROUNDUP(L82*$E83,0)</f>
+        <v>149</v>
+      </c>
+      <c r="M83" s="9" t="n">
+        <f aca="false">ROUNDUP(M82*$E83,0)</f>
+        <v>72</v>
+      </c>
+      <c r="N83" s="9" t="n">
+        <f aca="false">ROUNDUP(N82*$E83,0)</f>
+        <v>88</v>
+      </c>
+      <c r="O83" s="9" t="n">
+        <f aca="false">ROUNDUP(O82*$E83,0)</f>
+        <v>105</v>
+      </c>
+      <c r="P83" s="9" t="n">
+        <f aca="false">ROUNDUP(P82*$E83,0)</f>
+        <v>60</v>
+      </c>
+      <c r="Q83" s="9" t="n">
+        <f aca="false">ROUNDUP(Q82*$E83,0)</f>
+        <v>60</v>
+      </c>
+      <c r="R83" s="9" t="n">
+        <f aca="false">ROUNDUP(R82*$E83,0)</f>
+        <v>64</v>
+      </c>
+      <c r="S83" s="9" t="n">
+        <f aca="false">ROUNDUP(S82*$E83,0)</f>
+        <v>91</v>
+      </c>
+      <c r="T83" s="9" t="n">
+        <f aca="false">ROUNDUP(T82*$E83,0)</f>
+        <v>68</v>
+      </c>
+      <c r="U83" s="9" t="n">
+        <f aca="false">ROUNDUP(U82*$E83,0)</f>
+        <v>82</v>
+      </c>
+      <c r="V83" s="9" t="n">
+        <f aca="false">ROUNDUP(V82*$E83,0)</f>
+        <v>60</v>
+      </c>
+      <c r="W83" s="9" t="n">
+        <f aca="false">ROUNDUP(W82*$E83,0)</f>
+        <v>66</v>
+      </c>
+      <c r="X83" s="9" t="n">
+        <f aca="false">ROUNDUP(X82*$E83,0)</f>
+        <v>91</v>
+      </c>
+      <c r="Y83" s="9" t="n">
+        <f aca="false">ROUNDUP(Y82*$E83,0)</f>
+        <v>84</v>
+      </c>
+      <c r="Z83" s="9" t="n">
+        <f aca="false">ROUNDUP(Z82*$E83,0)</f>
+        <v>82</v>
+      </c>
+      <c r="AA83" s="9" t="n">
+        <f aca="false">ROUNDUP(AA82*$E83,0)</f>
         <v>124</v>
       </c>
-      <c r="D79" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E79" s="9" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G79" s="9" t="n">
-        <f aca="false">ROUNDUP(G80*E79,0)</f>
-        <v>230</v>
-      </c>
-      <c r="H79" s="9" t="n">
-        <f aca="false">ROUNDUP(H80*$E79,0)</f>
-        <v>117</v>
-      </c>
-      <c r="I79" s="9" t="n">
-        <f aca="false">ROUNDUP(I80*$E79,0)</f>
-        <v>117</v>
-      </c>
-      <c r="J79" s="9" t="n">
-        <f aca="false">ROUNDUP(J80*$E79,0)</f>
-        <v>144</v>
-      </c>
-      <c r="K79" s="9" t="n">
-        <f aca="false">ROUNDUP(K80*$E79,0)</f>
-        <v>113</v>
-      </c>
-      <c r="L79" s="9" t="n">
-        <f aca="false">ROUNDUP(L80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M79" s="9" t="n">
-        <f aca="false">ROUNDUP(M80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N79" s="9" t="n">
-        <f aca="false">ROUNDUP(N80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O79" s="9" t="n">
-        <f aca="false">ROUNDUP(O80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P79" s="9" t="n">
-        <f aca="false">ROUNDUP(P80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q79" s="9" t="n">
-        <f aca="false">ROUNDUP(Q80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R79" s="9" t="n">
-        <f aca="false">ROUNDUP(R80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="S79" s="9" t="n">
-        <f aca="false">ROUNDUP(S80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T79" s="9" t="n">
-        <f aca="false">ROUNDUP(T80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U79" s="9" t="n">
-        <f aca="false">ROUNDUP(U80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V79" s="9" t="n">
-        <f aca="false">ROUNDUP(V80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W79" s="9" t="n">
-        <f aca="false">ROUNDUP(W80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="X79" s="9" t="n">
-        <f aca="false">ROUNDUP(X80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y79" s="9" t="n">
-        <f aca="false">ROUNDUP(Y80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z79" s="9" t="n">
-        <f aca="false">ROUNDUP(Z80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA79" s="9" t="n">
-        <f aca="false">ROUNDUP(AA80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB79" s="9" t="n">
-        <f aca="false">ROUNDUP(AB80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC79" s="9" t="n">
-        <f aca="false">ROUNDUP(AC80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD79" s="9" t="n">
-        <f aca="false">ROUNDUP(AD80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE79" s="9" t="n">
-        <f aca="false">ROUNDUP(AE80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF79" s="9" t="n">
-        <f aca="false">ROUNDUP(AF80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AG79" s="9" t="n">
-        <f aca="false">ROUNDUP(AG80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH79" s="9" t="n">
-        <f aca="false">ROUNDUP(AH80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI79" s="9" t="n">
-        <f aca="false">ROUNDUP(AI80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ79" s="9" t="n">
-        <f aca="false">ROUNDUP(AJ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AK79" s="9" t="n">
-        <f aca="false">ROUNDUP(AK80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AL79" s="9" t="n">
-        <f aca="false">ROUNDUP(AL80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AM79" s="9" t="n">
-        <f aca="false">ROUNDUP(AM80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AN79" s="9" t="n">
-        <f aca="false">ROUNDUP(AN80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO79" s="9" t="n">
-        <f aca="false">ROUNDUP(AO80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP79" s="9" t="n">
-        <f aca="false">ROUNDUP(AP80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ79" s="9" t="n">
-        <f aca="false">ROUNDUP(AQ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AR79" s="9" t="n">
-        <f aca="false">ROUNDUP(AR80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AS79" s="9" t="n">
-        <f aca="false">ROUNDUP(AS80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AT79" s="9" t="n">
-        <f aca="false">ROUNDUP(AT80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AU79" s="9" t="n">
-        <f aca="false">ROUNDUP(AU80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AV79" s="9" t="n">
-        <f aca="false">ROUNDUP(AV80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AW79" s="9" t="n">
-        <f aca="false">ROUNDUP(AW80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AX79" s="9" t="n">
-        <f aca="false">ROUNDUP(AX80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AY79" s="9" t="n">
-        <f aca="false">ROUNDUP(AY80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ79" s="9" t="n">
-        <f aca="false">ROUNDUP(AZ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BA79" s="9" t="n">
-        <f aca="false">ROUNDUP(BA80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BB79" s="9" t="n">
-        <f aca="false">ROUNDUP(BB80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BC79" s="9" t="n">
-        <f aca="false">ROUNDUP(BC80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD79" s="9" t="n">
-        <f aca="false">ROUNDUP(BD80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BE79" s="9" t="n">
-        <f aca="false">ROUNDUP(BE80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BF79" s="9" t="n">
-        <f aca="false">ROUNDUP(BF80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BG79" s="9" t="n">
-        <f aca="false">ROUNDUP(BG80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BH79" s="9" t="n">
-        <f aca="false">ROUNDUP(BH80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BI79" s="9" t="n">
-        <f aca="false">ROUNDUP(BI80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ79" s="9" t="n">
-        <f aca="false">ROUNDUP(BJ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BK79" s="9" t="n">
-        <f aca="false">ROUNDUP(BK80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BL79" s="9" t="n">
-        <f aca="false">ROUNDUP(BL80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BM79" s="9" t="n">
-        <f aca="false">ROUNDUP(BM80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BN79" s="9" t="n">
-        <f aca="false">ROUNDUP(BN80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BO79" s="9" t="n">
-        <f aca="false">ROUNDUP(BO80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BP79" s="9" t="n">
-        <f aca="false">ROUNDUP(BP80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ79" s="9" t="n">
-        <f aca="false">ROUNDUP(BQ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BR79" s="9" t="n">
-        <f aca="false">ROUNDUP(BR80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BS79" s="9" t="n">
-        <f aca="false">ROUNDUP(BS80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BT79" s="9" t="n">
-        <f aca="false">ROUNDUP(BT80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BU79" s="9" t="n">
-        <f aca="false">ROUNDUP(BU80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BV79" s="9" t="n">
-        <f aca="false">ROUNDUP(BV80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BW79" s="9" t="n">
-        <f aca="false">ROUNDUP(BW80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BX79" s="9" t="n">
-        <f aca="false">ROUNDUP(BX80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BY79" s="9" t="n">
-        <f aca="false">ROUNDUP(BY80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BZ79" s="9" t="n">
-        <f aca="false">ROUNDUP(BZ80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CA79" s="9" t="n">
-        <f aca="false">ROUNDUP(CA80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CB79" s="9" t="n">
-        <f aca="false">ROUNDUP(CB80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CC79" s="9" t="n">
-        <f aca="false">ROUNDUP(CC80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CD79" s="9" t="n">
-        <f aca="false">ROUNDUP(CD80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CE79" s="9" t="n">
-        <f aca="false">ROUNDUP(CE80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CF79" s="9" t="n">
-        <f aca="false">ROUNDUP(CF80*$E79,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CG79" s="9" t="n">
-        <f aca="false">ROUNDUP(CG80*$E79,0)</f>
+      <c r="AB83" s="9" t="n">
+        <f aca="false">ROUNDUP(AB82*$E83,0)</f>
+        <v>157</v>
+      </c>
+      <c r="AC83" s="9" t="n">
+        <f aca="false">ROUNDUP(AC82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD83" s="9" t="n">
+        <f aca="false">ROUNDUP(AD82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE83" s="9" t="n">
+        <f aca="false">ROUNDUP(AE82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF83" s="9" t="n">
+        <f aca="false">ROUNDUP(AF82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG83" s="9" t="n">
+        <f aca="false">ROUNDUP(AG82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH83" s="9" t="n">
+        <f aca="false">ROUNDUP(AH82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI83" s="9" t="n">
+        <f aca="false">ROUNDUP(AI82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="9" t="n">
+        <f aca="false">ROUNDUP(AJ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AK83" s="9" t="n">
+        <f aca="false">ROUNDUP(AK82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AL83" s="9" t="n">
+        <f aca="false">ROUNDUP(AL82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AM83" s="9" t="n">
+        <f aca="false">ROUNDUP(AM82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN83" s="9" t="n">
+        <f aca="false">ROUNDUP(AN82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO83" s="9" t="n">
+        <f aca="false">ROUNDUP(AO82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP83" s="9" t="n">
+        <f aca="false">ROUNDUP(AP82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ83" s="9" t="n">
+        <f aca="false">ROUNDUP(AQ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR83" s="9" t="n">
+        <f aca="false">ROUNDUP(AR82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AS83" s="9" t="n">
+        <f aca="false">ROUNDUP(AS82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AT83" s="9" t="n">
+        <f aca="false">ROUNDUP(AT82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AU83" s="9" t="n">
+        <f aca="false">ROUNDUP(AU82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AV83" s="9" t="n">
+        <f aca="false">ROUNDUP(AV82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AW83" s="9" t="n">
+        <f aca="false">ROUNDUP(AW82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX83" s="9" t="n">
+        <f aca="false">ROUNDUP(AX82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AY83" s="9" t="n">
+        <f aca="false">ROUNDUP(AY82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ83" s="9" t="n">
+        <f aca="false">ROUNDUP(AZ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BA83" s="9" t="n">
+        <f aca="false">ROUNDUP(BA82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BB83" s="9" t="n">
+        <f aca="false">ROUNDUP(BB82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BC83" s="9" t="n">
+        <f aca="false">ROUNDUP(BC82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BD83" s="9" t="n">
+        <f aca="false">ROUNDUP(BD82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BE83" s="9" t="n">
+        <f aca="false">ROUNDUP(BE82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BF83" s="9" t="n">
+        <f aca="false">ROUNDUP(BF82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BG83" s="9" t="n">
+        <f aca="false">ROUNDUP(BG82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BH83" s="9" t="n">
+        <f aca="false">ROUNDUP(BH82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BI83" s="9" t="n">
+        <f aca="false">ROUNDUP(BI82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ83" s="9" t="n">
+        <f aca="false">ROUNDUP(BJ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BK83" s="9" t="n">
+        <f aca="false">ROUNDUP(BK82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BL83" s="9" t="n">
+        <f aca="false">ROUNDUP(BL82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BM83" s="9" t="n">
+        <f aca="false">ROUNDUP(BM82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BN83" s="9" t="n">
+        <f aca="false">ROUNDUP(BN82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BO83" s="9" t="n">
+        <f aca="false">ROUNDUP(BO82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BP83" s="9" t="n">
+        <f aca="false">ROUNDUP(BP82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ83" s="9" t="n">
+        <f aca="false">ROUNDUP(BQ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BR83" s="9" t="n">
+        <f aca="false">ROUNDUP(BR82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BS83" s="9" t="n">
+        <f aca="false">ROUNDUP(BS82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BT83" s="9" t="n">
+        <f aca="false">ROUNDUP(BT82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BU83" s="9" t="n">
+        <f aca="false">ROUNDUP(BU82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BV83" s="9" t="n">
+        <f aca="false">ROUNDUP(BV82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BW83" s="9" t="n">
+        <f aca="false">ROUNDUP(BW82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BX83" s="9" t="n">
+        <f aca="false">ROUNDUP(BX82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BY83" s="9" t="n">
+        <f aca="false">ROUNDUP(BY82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ83" s="9" t="n">
+        <f aca="false">ROUNDUP(BZ82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CA83" s="9" t="n">
+        <f aca="false">ROUNDUP(CA82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CB83" s="9" t="n">
+        <f aca="false">ROUNDUP(CB82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CC83" s="9" t="n">
+        <f aca="false">ROUNDUP(CC82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CD83" s="9" t="n">
+        <f aca="false">ROUNDUP(CD82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CE83" s="9" t="n">
+        <f aca="false">ROUNDUP(CE82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CF83" s="9" t="n">
+        <f aca="false">ROUNDUP(CF82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CG83" s="9" t="n">
+        <f aca="false">ROUNDUP(CG82*$E83,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CH83" s="9" t="n">
+        <f aca="false">ROUNDUP(CH82*$E83,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E80" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(G6:G78, E6:E78)</f>
-        <v>255</v>
-      </c>
-      <c r="H80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(H6:H78, $E6:$E78)</f>
-        <v>130</v>
-      </c>
-      <c r="I80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(I6:I78, $E6:$E78)</f>
-        <v>130</v>
-      </c>
-      <c r="J80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(J6:J78, $E6:$E78)</f>
-        <v>160</v>
-      </c>
-      <c r="K80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(K6:K78, $E6:$E78)</f>
-        <v>125</v>
-      </c>
-      <c r="L80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(L6:L78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="M80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(M6:M78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="N80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(N6:N78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="O80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(O6:O78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="P80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(P6:P78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="Q80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(Q6:Q78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="R80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(R6:R78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="S80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(S6:S78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="T80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(T6:T78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="U80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(U6:U78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="V80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(V6:V78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="W80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(W6:W78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="X80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(X6:X78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="Y80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(Y6:Y78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="Z80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(Z6:Z78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AA80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AA6:AA78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AB80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AB6:AB78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AC80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AC6:AC78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AD80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AD6:AD78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AE80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AE6:AE78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AF80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AF6:AF78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AG80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AG6:AG78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AH80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AH6:AH78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AI80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AI6:AI78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AJ6:AJ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AK80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AK6:AK78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AL80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AL6:AL78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AM80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AM6:AM78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AN80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AN6:AN78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AO80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AO6:AO78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AP80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AP6:AP78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AQ6:AQ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AR80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AR6:AR78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AS80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AS6:AS78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AT80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AT6:AT78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AU80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AU6:AU78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AV80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AV6:AV78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AW80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AW6:AW78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AX80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AX6:AX78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AY80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AY6:AY78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(AZ6:AZ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BA80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BA6:BA78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BB80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BB6:BB78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BC80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BC6:BC78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BD80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BD6:BD78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BE80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BE6:BE78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BF80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BF6:BF78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BG80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BG6:BG78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BH80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BH6:BH78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BI80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BI6:BI78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BJ6:BJ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BK80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BK6:BK78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BL80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BL6:BL78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BM80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BM6:BM78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BN80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BN6:BN78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BO80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BO6:BO78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BP80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BP6:BP78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BQ6:BQ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BR80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BR6:BR78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BS80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BS6:BS78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BT80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BT6:BT78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BU80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BU6:BU78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BV80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BV6:BV78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BW80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BW6:BW78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BX80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BX6:BX78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BY80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BY6:BY78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="BZ80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(BZ6:BZ78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CA80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CA6:CA78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CB80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CB6:CB78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CC80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CC6:CC78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CD80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CD6:CD78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CE80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CE6:CE78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CF80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CF6:CF78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-      <c r="CG80" s="9" t="n">
-        <f aca="false">SUMPRODUCT(CG6:CG78, $E6:$E78)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E81" s="9" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="G81" s="9" t="n">
-        <f aca="false">ROUNDUP(G80*E81,0)</f>
-        <v>281</v>
-      </c>
-      <c r="H81" s="9" t="n">
-        <f aca="false">ROUNDUP(H80*$E81,0)</f>
-        <v>143</v>
-      </c>
-      <c r="I81" s="9" t="n">
-        <f aca="false">ROUNDUP(I80*$E81,0)</f>
-        <v>143</v>
-      </c>
-      <c r="J81" s="9" t="n">
-        <f aca="false">ROUNDUP(J80*$E81,0)</f>
-        <v>176</v>
-      </c>
-      <c r="K81" s="9" t="n">
-        <f aca="false">ROUNDUP(K80*$E81,0)</f>
-        <v>138</v>
-      </c>
-      <c r="L81" s="9" t="n">
-        <f aca="false">ROUNDUP(L80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M81" s="9" t="n">
-        <f aca="false">ROUNDUP(M80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N81" s="9" t="n">
-        <f aca="false">ROUNDUP(N80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O81" s="9" t="n">
-        <f aca="false">ROUNDUP(O80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P81" s="9" t="n">
-        <f aca="false">ROUNDUP(P80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q81" s="9" t="n">
-        <f aca="false">ROUNDUP(Q80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R81" s="9" t="n">
-        <f aca="false">ROUNDUP(R80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="S81" s="9" t="n">
-        <f aca="false">ROUNDUP(S80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T81" s="9" t="n">
-        <f aca="false">ROUNDUP(T80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U81" s="9" t="n">
-        <f aca="false">ROUNDUP(U80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V81" s="9" t="n">
-        <f aca="false">ROUNDUP(V80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W81" s="9" t="n">
-        <f aca="false">ROUNDUP(W80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="X81" s="9" t="n">
-        <f aca="false">ROUNDUP(X80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y81" s="9" t="n">
-        <f aca="false">ROUNDUP(Y80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z81" s="9" t="n">
-        <f aca="false">ROUNDUP(Z80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA81" s="9" t="n">
-        <f aca="false">ROUNDUP(AA80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB81" s="9" t="n">
-        <f aca="false">ROUNDUP(AB80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC81" s="9" t="n">
-        <f aca="false">ROUNDUP(AC80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD81" s="9" t="n">
-        <f aca="false">ROUNDUP(AD80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE81" s="9" t="n">
-        <f aca="false">ROUNDUP(AE80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF81" s="9" t="n">
-        <f aca="false">ROUNDUP(AF80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AG81" s="9" t="n">
-        <f aca="false">ROUNDUP(AG80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH81" s="9" t="n">
-        <f aca="false">ROUNDUP(AH80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI81" s="9" t="n">
-        <f aca="false">ROUNDUP(AI80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ81" s="9" t="n">
-        <f aca="false">ROUNDUP(AJ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AK81" s="9" t="n">
-        <f aca="false">ROUNDUP(AK80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AL81" s="9" t="n">
-        <f aca="false">ROUNDUP(AL80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AM81" s="9" t="n">
-        <f aca="false">ROUNDUP(AM80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AN81" s="9" t="n">
-        <f aca="false">ROUNDUP(AN80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO81" s="9" t="n">
-        <f aca="false">ROUNDUP(AO80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP81" s="9" t="n">
-        <f aca="false">ROUNDUP(AP80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ81" s="9" t="n">
-        <f aca="false">ROUNDUP(AQ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AR81" s="9" t="n">
-        <f aca="false">ROUNDUP(AR80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AS81" s="9" t="n">
-        <f aca="false">ROUNDUP(AS80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AT81" s="9" t="n">
-        <f aca="false">ROUNDUP(AT80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AU81" s="9" t="n">
-        <f aca="false">ROUNDUP(AU80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AV81" s="9" t="n">
-        <f aca="false">ROUNDUP(AV80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AW81" s="9" t="n">
-        <f aca="false">ROUNDUP(AW80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AX81" s="9" t="n">
-        <f aca="false">ROUNDUP(AX80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AY81" s="9" t="n">
-        <f aca="false">ROUNDUP(AY80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ81" s="9" t="n">
-        <f aca="false">ROUNDUP(AZ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BA81" s="9" t="n">
-        <f aca="false">ROUNDUP(BA80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BB81" s="9" t="n">
-        <f aca="false">ROUNDUP(BB80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BC81" s="9" t="n">
-        <f aca="false">ROUNDUP(BC80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD81" s="9" t="n">
-        <f aca="false">ROUNDUP(BD80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BE81" s="9" t="n">
-        <f aca="false">ROUNDUP(BE80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BF81" s="9" t="n">
-        <f aca="false">ROUNDUP(BF80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BG81" s="9" t="n">
-        <f aca="false">ROUNDUP(BG80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BH81" s="9" t="n">
-        <f aca="false">ROUNDUP(BH80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BI81" s="9" t="n">
-        <f aca="false">ROUNDUP(BI80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ81" s="9" t="n">
-        <f aca="false">ROUNDUP(BJ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BK81" s="9" t="n">
-        <f aca="false">ROUNDUP(BK80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BL81" s="9" t="n">
-        <f aca="false">ROUNDUP(BL80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BM81" s="9" t="n">
-        <f aca="false">ROUNDUP(BM80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BN81" s="9" t="n">
-        <f aca="false">ROUNDUP(BN80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BO81" s="9" t="n">
-        <f aca="false">ROUNDUP(BO80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BP81" s="9" t="n">
-        <f aca="false">ROUNDUP(BP80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ81" s="9" t="n">
-        <f aca="false">ROUNDUP(BQ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BR81" s="9" t="n">
-        <f aca="false">ROUNDUP(BR80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BS81" s="9" t="n">
-        <f aca="false">ROUNDUP(BS80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BT81" s="9" t="n">
-        <f aca="false">ROUNDUP(BT80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BU81" s="9" t="n">
-        <f aca="false">ROUNDUP(BU80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BV81" s="9" t="n">
-        <f aca="false">ROUNDUP(BV80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BW81" s="9" t="n">
-        <f aca="false">ROUNDUP(BW80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BX81" s="9" t="n">
-        <f aca="false">ROUNDUP(BX80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BY81" s="9" t="n">
-        <f aca="false">ROUNDUP(BY80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="BZ81" s="9" t="n">
-        <f aca="false">ROUNDUP(BZ80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CA81" s="9" t="n">
-        <f aca="false">ROUNDUP(CA80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CB81" s="9" t="n">
-        <f aca="false">ROUNDUP(CB80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CC81" s="9" t="n">
-        <f aca="false">ROUNDUP(CC80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CD81" s="9" t="n">
-        <f aca="false">ROUNDUP(CD80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CE81" s="9" t="n">
-        <f aca="false">ROUNDUP(CE80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CF81" s="9" t="n">
-        <f aca="false">ROUNDUP(CF80*$E81,0)</f>
-        <v>0</v>
-      </c>
-      <c r="CG81" s="9" t="n">
-        <f aca="false">ROUNDUP(CG80*$E81,0)</f>
-        <v>0</v>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M87" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -10627,11 +11020,11 @@
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="C11:C17"/>
     <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C23:C57"/>
+    <mergeCell ref="C23:C58"/>
     <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C62:C73"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C79:C81"/>
+    <mergeCell ref="C62:C75"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C81:C83"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>